<commit_message>
- Earcons - TTS spell incoming number - Deal with private numbers
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>Task</t>
   </si>
@@ -36,12 +36,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Lidar com pop-up menu após chamada</t>
-  </si>
-  <si>
-    <t>TTS spell function</t>
-  </si>
-  <si>
     <t>Usar lista de contactos em incoming call</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
     <t>No segundo ciclo de leitura não permite escolha da ultima opção</t>
   </si>
   <si>
-    <t>Debug todas as combinações de chamadas</t>
-  </si>
-  <si>
     <t>debug</t>
   </si>
   <si>
@@ -75,9 +66,6 @@
     <t>Status (Done, Discarded, TBD, Wish)</t>
   </si>
   <si>
-    <t>Increase InCall TTS volume</t>
-  </si>
-  <si>
     <t>TBD</t>
   </si>
   <si>
@@ -103,6 +91,24 @@
   </si>
   <si>
     <t>modification</t>
+  </si>
+  <si>
+    <t>Hugo</t>
+  </si>
+  <si>
+    <t>TTS Spell</t>
+  </si>
+  <si>
+    <t>Lidar com numero privado (incoming number = null)</t>
+  </si>
+  <si>
+    <t>Lidar com pop-up menu após chamada (só vodafone?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug todas as combinações de fazer chamada </t>
+  </si>
+  <si>
+    <t>Debug todas as combinações de receber chamada / em chamada</t>
   </si>
 </sst>
 </file>
@@ -550,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -572,13 +578,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -592,170 +598,208 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B4" s="5">
         <v>2</v>
       </c>
+      <c r="C4" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5">
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="5">
         <v>3</v>
       </c>
+      <c r="C6" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="D6" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5">
         <v>3</v>
       </c>
+      <c r="C7" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="D7" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B8" s="8">
-        <v>2</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>26</v>
+        <v>3</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B9" s="5">
         <v>2</v>
       </c>
+      <c r="C9" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="D9" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
       </c>
+      <c r="C10" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="D10" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="5">
         <v>1</v>
       </c>
+      <c r="C11" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="D11" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" s="8">
         <v>1</v>
       </c>
+      <c r="C12" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="D12" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="8">
+        <v>2</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1">
-    <sortState ref="A2:G12">
+    <sortState ref="A2:G13">
       <sortCondition descending="1" ref="D1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
- Utils.java added - Get contactName added - Set Speakerphone On when In Call
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>Task</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>Debug todas as combinações de receber chamada / em chamada</t>
+  </si>
+  <si>
+    <t>Se não existir auricular ligar altifalante</t>
+  </si>
+  <si>
+    <t>Usar lista de contactos no easyphone</t>
+  </si>
+  <si>
+    <t>Ligar altifalante</t>
   </si>
 </sst>
 </file>
@@ -556,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -646,41 +655,29 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="5">
+        <v>31</v>
+      </c>
+      <c r="B5" s="8">
         <v>3</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="5">
-        <v>3</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>7</v>
+        <v>30</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B7" s="5">
         <v>3</v>
@@ -697,27 +694,30 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5">
         <v>3</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="8" t="s">
+      <c r="C8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>22</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B9" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>24</v>
@@ -726,35 +726,32 @@
         <v>16</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="5">
-        <v>1</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="B10" s="8">
+        <v>3</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B11" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>24</v>
@@ -763,43 +760,94 @@
         <v>16</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5">
         <v>1</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>23</v>
+      <c r="C12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="8">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B15" s="8">
         <v>2</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="8" t="s">
+      <c r="C15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1">
-    <sortState ref="A2:G13">
+    <sortState ref="A2:G16">
       <sortCondition descending="1" ref="D1"/>
     </sortState>
   </autoFilter>

</xml_diff>